<commit_message>
Reading locators from excel file now. Added one demo test to run
</commit_message>
<xml_diff>
--- a/OR/Locator.xlsx
+++ b/OR/Locator.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="45">
   <si>
     <t>PageName</t>
   </si>
@@ -92,6 +92,69 @@
   </si>
   <si>
     <t>Diagnostic</t>
+  </si>
+  <si>
+    <t>News</t>
+  </si>
+  <si>
+    <t>Textbox</t>
+  </si>
+  <si>
+    <t>//label[contains(text(),"Title")]/following-sibling::input</t>
+  </si>
+  <si>
+    <t>//b[contains(text(),'Summary')]//..//..//textarea[@class='pt-input pt-fixed']</t>
+  </si>
+  <si>
+    <t>Textarea</t>
+  </si>
+  <si>
+    <t>//label[contains(.,"Body")]//following::div[@class='id-froala']//div[@contenteditable='true']</t>
+  </si>
+  <si>
+    <t>Button</t>
+  </si>
+  <si>
+    <t>//div[@class='pt-fill' and contains(text(),"Submit Article")]</t>
+  </si>
+  <si>
+    <t>//div[@class='id-form__footer']/button[@type='button']</t>
+  </si>
+  <si>
+    <t>NewsSubmissionPage.NewsTitle</t>
+  </si>
+  <si>
+    <t>NewsSubmissionPage.NewsSummary</t>
+  </si>
+  <si>
+    <t>NewsSubmissionPage.NewsBody</t>
+  </si>
+  <si>
+    <t>NewsSubmissionPage.NewsSubmitArticle</t>
+  </si>
+  <si>
+    <t>NewsSubmissionPage.NewsSubmit</t>
+  </si>
+  <si>
+    <t>FrontEndLoginButton</t>
+  </si>
+  <si>
+    <t>//*[@id="btnLogin"]</t>
+  </si>
+  <si>
+    <t>FrontEndPasswordTextBox</t>
+  </si>
+  <si>
+    <t>FrontEndUsernameTextBox</t>
+  </si>
+  <si>
+    <t>//*[@id="textPassword"]</t>
+  </si>
+  <si>
+    <t>//*[@id="textUsername"]</t>
+  </si>
+  <si>
+    <t>FrontEndLogin</t>
   </si>
 </sst>
 </file>
@@ -571,13 +634,13 @@
   <dimension ref="A1:E281"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="40.6328125" customWidth="1"/>
-    <col min="2" max="2" width="52.7265625" customWidth="1"/>
+    <col min="2" max="2" width="38.1796875" customWidth="1"/>
     <col min="3" max="3" width="24.08984375" customWidth="1"/>
     <col min="4" max="4" width="76.453125" customWidth="1"/>
     <col min="5" max="5" width="51" customWidth="1"/>
@@ -598,53 +661,117 @@
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A2" s="2"/>
-      <c r="B2" s="2"/>
-      <c r="C2" s="2"/>
-      <c r="D2" s="2"/>
+      <c r="A2" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A3" s="2"/>
-      <c r="B3" s="2"/>
-      <c r="C3" s="2"/>
-      <c r="D3" s="2"/>
+      <c r="A3" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A4" s="2"/>
-      <c r="B4" s="2"/>
-      <c r="C4" s="2"/>
-      <c r="D4" s="2"/>
+      <c r="A4" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A5" s="2"/>
-      <c r="B5" s="2"/>
-      <c r="C5" s="2"/>
-      <c r="D5" s="2"/>
+      <c r="A5" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>31</v>
+      </c>
       <c r="E5" s="18"/>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A6" s="2"/>
-      <c r="B6" s="2"/>
-      <c r="C6" s="2"/>
-      <c r="D6" s="2"/>
+      <c r="A6" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A7" s="2"/>
-      <c r="B7" s="2"/>
-      <c r="C7" s="2"/>
-      <c r="D7" s="2"/>
+      <c r="A7" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>39</v>
+      </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A8" s="2"/>
-      <c r="B8" s="2"/>
-      <c r="C8" s="2"/>
-      <c r="D8" s="2"/>
+      <c r="A8" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="D8" t="s">
+        <v>42</v>
+      </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A9" s="2"/>
-      <c r="B9" s="2"/>
-      <c r="C9" s="2"/>
-      <c r="D9" s="2"/>
+      <c r="A9" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>43</v>
+      </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A10" s="2"/>

</xml_diff>